<commit_message>
configured configurable hierarchy for health facility, patient service delivery group, patient contact, and facility employee
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/health_facility-create.xlsx
+++ b/config/default/forms/contact/health_facility-create.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="217">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -465,24 +465,6 @@
     <t xml:space="preserve">Staff médical</t>
   </si>
   <si>
-    <t xml:space="preserve">patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient</t>
-  </si>
-  <si>
-    <t xml:space="preserve">मरीज़ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pasien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mgonjwa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">बिरामी</t>
-  </si>
-  <si>
     <t xml:space="preserve">kp_case_manager</t>
   </si>
   <si>
@@ -505,24 +487,6 @@
   </si>
   <si>
     <t xml:space="preserve">Clinician</t>
-  </si>
-  <si>
-    <t xml:space="preserve">other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">अन्य</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nyingine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Autre</t>
   </si>
   <si>
     <t xml:space="preserve">yes_no_generated_name</t>
@@ -1583,29 +1547,26 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="L15" activeCellId="0" sqref="L15"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.719387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.4183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.9285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.3367346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.719387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.3979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.9183673469388"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="79.1938775510204"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.1683673469388"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.9489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.7244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="58.4081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.3469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.8367346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="81.984693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.8979591836735"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.1581632653061"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="33.0255102040816"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2671,20 +2632,22 @@
   <dimension ref="A1:Z65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.3163265306123"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.3265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="27.3571428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.45918367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="8.45918367346939"/>
-    <col collapsed="false" hidden="false" max="26" min="14" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.2091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.6683673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.4081632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="26" min="14" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3211,28 +3174,18 @@
       <c r="A13" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>152</v>
-      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
       <c r="H13" s="19"/>
-      <c r="I13" s="20" t="s">
-        <v>148</v>
-      </c>
+      <c r="I13" s="20"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
@@ -3256,10 +3209,10 @@
         <v>119</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="22"/>
@@ -3290,10 +3243,10 @@
         <v>119</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="22"/>
@@ -3324,10 +3277,10 @@
         <v>119</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="22"/>
@@ -3354,21 +3307,31 @@
       <c r="Z16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>159</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
+      <c r="A17" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="H17" s="19"/>
-      <c r="I17" s="20"/>
+      <c r="I17" s="20" t="s">
+        <v>79</v>
+      </c>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
@@ -3388,30 +3351,30 @@
       <c r="Z17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B18" s="23" t="s">
+      <c r="A18" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="G18" s="18" t="s">
         <v>161</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>163</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="20" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
@@ -3432,30 +3395,30 @@
       <c r="Z18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="E19" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="B19" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>76</v>
-      </c>
       <c r="F19" s="17" t="s">
-        <v>77</v>
+        <v>168</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="20" t="s">
-        <v>79</v>
+        <v>170</v>
       </c>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
@@ -3476,30 +3439,30 @@
       <c r="Z19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>169</v>
+      <c r="A20" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>172</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="20" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
@@ -3521,29 +3484,29 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F21" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="G21" s="18" t="s">
         <v>180</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>181</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="20" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
@@ -3565,29 +3528,29 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="13" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="D22" s="15" t="s">
         <v>185</v>
       </c>
+      <c r="D22" s="25" t="s">
+        <v>186</v>
+      </c>
       <c r="E22" s="22" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F22" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="G22" s="18" t="s">
         <v>188</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>189</v>
       </c>
       <c r="H22" s="19"/>
       <c r="I22" s="20" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
@@ -3609,15 +3572,15 @@
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="13" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="C23" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="25" t="s">
         <v>192</v>
       </c>
       <c r="E23" s="22" t="s">
@@ -3626,12 +3589,12 @@
       <c r="F23" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="G23" s="18" t="s">
-        <v>192</v>
+      <c r="G23" s="26" t="s">
+        <v>195</v>
       </c>
       <c r="H23" s="19"/>
       <c r="I23" s="20" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
@@ -3653,10 +3616,10 @@
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C24" s="24" t="s">
         <v>197</v>
@@ -3670,7 +3633,7 @@
       <c r="F24" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="G24" s="26" t="s">
+      <c r="G24" s="27" t="s">
         <v>201</v>
       </c>
       <c r="H24" s="19"/>
@@ -3696,16 +3659,16 @@
       <c r="Z24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13" t="s">
-        <v>196</v>
+      <c r="A25" s="28" t="s">
+        <v>203</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="D25" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="15" t="s">
         <v>204</v>
       </c>
       <c r="E25" s="22" t="s">
@@ -3714,12 +3677,12 @@
       <c r="F25" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="G25" s="26" t="s">
-        <v>207</v>
+      <c r="G25" s="18" t="s">
+        <v>204</v>
       </c>
       <c r="H25" s="19"/>
       <c r="I25" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
@@ -3739,94 +3702,8 @@
       <c r="Y25" s="13"/>
       <c r="Z25" s="13"/>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="C26" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>210</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="F26" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="G26" s="27" t="s">
-        <v>213</v>
-      </c>
-      <c r="H26" s="19"/>
-      <c r="I26" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13"/>
-      <c r="U26" s="13"/>
-      <c r="V26" s="13"/>
-      <c r="W26" s="13"/>
-      <c r="X26" s="13"/>
-      <c r="Y26" s="13"/>
-      <c r="Z26" s="13"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>217</v>
-      </c>
-      <c r="F27" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="G27" s="18" t="s">
-        <v>216</v>
-      </c>
-      <c r="H27" s="19"/>
-      <c r="I27" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="13"/>
-      <c r="V27" s="13"/>
-      <c r="W27" s="13"/>
-      <c r="X27" s="13"/>
-      <c r="Y27" s="13"/>
-      <c r="Z27" s="13"/>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3852,32 +3729,33 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.7091836734694"/>
-    <col collapsed="false" hidden="false" max="14" min="7" style="0" width="8.45918367346939"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.780612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.38775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.0561224489796"/>
+    <col collapsed="false" hidden="false" max="14" min="7" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="29" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="F1" s="29"/>
       <c r="G1" s="13"/>
@@ -3902,20 +3780,20 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="C2" s="30" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2020-09-25  22-37</v>
+        <v>2020-09-28  11-54</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>

</xml_diff>